<commit_message>
updated summary charts and summary reports including comments from Prof. Erhardt
updated summary charts and summary reports including comments from Prof. Erhardt
</commit_message>
<xml_diff>
--- a/Factors and Ridership Data/Script Outputs/Est7_Outputs/FAC Summary Reports/Albany, GA Metro Area-Bus.xlsx
+++ b/Factors and Ridership Data/Script Outputs/Est7_Outputs/FAC Summary Reports/Albany, GA Metro Area-Bus.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="28680" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -302,6 +302,24 @@
     <xf borderId="12" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="13" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="4" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="11" fillId="0" fontId="4" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="10" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -314,36 +332,12 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="13" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle builtinId="5" name="Percent" xfId="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -668,8 +662,8 @@
   </sheetPr>
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -694,7 +688,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>2012</t>
         </is>
       </c>
     </row>
@@ -711,7 +705,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="36" t="inlineStr">
+      <c r="B3" s="48" t="inlineStr">
         <is>
           <t>Factors affecting change</t>
         </is>
@@ -723,7 +717,7 @@
           <t>Dependent Variable</t>
         </is>
       </c>
-      <c r="C4" s="35" t="inlineStr">
+      <c r="C4" s="47" t="inlineStr">
         <is>
           <t>LN(Unlinked Passenger Trips)</t>
         </is>
@@ -745,14 +739,14 @@
         </is>
       </c>
       <c r="D6" s="33" t="n"/>
-      <c r="E6" s="34" t="inlineStr">
+      <c r="E6" s="46" t="inlineStr">
         <is>
           <t>Average Values</t>
         </is>
       </c>
       <c r="F6" s="3" t="n"/>
       <c r="G6" s="4" t="n"/>
-      <c r="H6" s="34" t="inlineStr">
+      <c r="H6" s="46" t="inlineStr">
         <is>
           <t>Riddership Effect</t>
         </is>
@@ -777,7 +771,7 @@
       </c>
       <c r="E7" s="23" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="F7" s="23" t="inlineStr">
@@ -814,21 +808,21 @@
         </is>
       </c>
       <c r="D8" s="33" t="n"/>
-      <c r="E8" s="33" t="n">
-        <v>532194</v>
-      </c>
-      <c r="F8" s="33" t="n">
+      <c r="E8" s="37" t="n">
+        <v>523493</v>
+      </c>
+      <c r="F8" s="37" t="n">
         <v>659043</v>
       </c>
-      <c r="G8" s="33">
-        <f>IFERROR((F8-E8)*100/E8,0)</f>
-        <v/>
-      </c>
-      <c r="H8" s="38" t="n">
-        <v>158677.5225779</v>
-      </c>
-      <c r="I8" s="33">
-        <f>IFERROR(H8*100/$E$21,0)</f>
+      <c r="G8" s="43">
+        <f>IFERROR((F8-E8)/E8,0)</f>
+        <v/>
+      </c>
+      <c r="H8" s="41" t="n">
+        <v>99898.475282</v>
+      </c>
+      <c r="I8" s="43">
+        <f>IFERROR(H8/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -844,21 +838,21 @@
         </is>
       </c>
       <c r="D9" s="33" t="n"/>
-      <c r="E9" s="33" t="n">
-        <v>0.6753121</v>
-      </c>
-      <c r="F9" s="33" t="n">
+      <c r="E9" s="37" t="n">
+        <v>0.56048164</v>
+      </c>
+      <c r="F9" s="37" t="n">
         <v>0.579495632</v>
       </c>
-      <c r="G9" s="33">
-        <f>IFERROR((F9-E9)*100/E9,0)</f>
-        <v/>
-      </c>
-      <c r="H9" s="38" t="n">
-        <v>1588.597734199997</v>
-      </c>
-      <c r="I9" s="33">
-        <f>IFERROR(H9*100/$E$21,0)</f>
+      <c r="G9" s="43">
+        <f>IFERROR((F9-E9)/E9,0)</f>
+        <v/>
+      </c>
+      <c r="H9" s="41" t="n">
+        <v>-33892.95714299999</v>
+      </c>
+      <c r="I9" s="43">
+        <f>IFERROR(H9/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -874,21 +868,21 @@
         </is>
       </c>
       <c r="D10" s="33" t="n"/>
-      <c r="E10" s="33" t="n">
-        <v>212581.0956</v>
-      </c>
-      <c r="F10" s="33" t="n">
+      <c r="E10" s="37" t="n">
+        <v>217565.42</v>
+      </c>
+      <c r="F10" s="37" t="n">
         <v>215656.43</v>
       </c>
-      <c r="G10" s="33">
-        <f>IFERROR((F10-E10)*100/E10,0)</f>
-        <v/>
-      </c>
-      <c r="H10" s="38" t="n">
-        <v>-5160.899603399997</v>
-      </c>
-      <c r="I10" s="33">
-        <f>IFERROR(H10*100/$E$21,0)</f>
+      <c r="G10" s="43">
+        <f>IFERROR((F10-E10)/E10,0)</f>
+        <v/>
+      </c>
+      <c r="H10" s="41" t="n">
+        <v>-14025.0092266</v>
+      </c>
+      <c r="I10" s="43">
+        <f>IFERROR(H10/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -900,21 +894,21 @@
       </c>
       <c r="C11" s="26" t="n"/>
       <c r="D11" s="33" t="n"/>
-      <c r="E11" s="33" t="n">
-        <v>1.896125531</v>
-      </c>
-      <c r="F11" s="33" t="n">
+      <c r="E11" s="37" t="n">
+        <v>1.040517614</v>
+      </c>
+      <c r="F11" s="37" t="n">
         <v>0.8451211040000001</v>
       </c>
-      <c r="G11" s="33">
-        <f>IFERROR((F11-E11)*100/E11,0)</f>
-        <v/>
-      </c>
-      <c r="H11" s="38" t="n">
-        <v>-3829.60943795</v>
-      </c>
-      <c r="I11" s="33">
-        <f>IFERROR(H11*100/$E$21,0)</f>
+      <c r="G11" s="43">
+        <f>IFERROR((F11-E11)/E11,0)</f>
+        <v/>
+      </c>
+      <c r="H11" s="41" t="n">
+        <v>270.8059292499999</v>
+      </c>
+      <c r="I11" s="43">
+        <f>IFERROR(H11/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -930,21 +924,21 @@
         </is>
       </c>
       <c r="D12" s="33" t="n"/>
-      <c r="E12" s="33" t="n">
-        <v>1.862</v>
-      </c>
-      <c r="F12" s="33" t="n">
+      <c r="E12" s="37" t="n">
+        <v>3.9458</v>
+      </c>
+      <c r="F12" s="37" t="n">
         <v>2.71</v>
       </c>
-      <c r="G12" s="33">
-        <f>IFERROR((F12-E12)*100/E12,0)</f>
-        <v/>
-      </c>
-      <c r="H12" s="38" t="n">
-        <v>22232.88644970002</v>
-      </c>
-      <c r="I12" s="33">
-        <f>IFERROR(H12*100/$E$21,0)</f>
+      <c r="G12" s="43">
+        <f>IFERROR((F12-E12)/E12,0)</f>
+        <v/>
+      </c>
+      <c r="H12" s="41" t="n">
+        <v>-47102.2481873</v>
+      </c>
+      <c r="I12" s="43">
+        <f>IFERROR(H12/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -960,21 +954,21 @@
         </is>
       </c>
       <c r="D13" s="33" t="n"/>
-      <c r="E13" s="33" t="n">
-        <v>32764.39688</v>
-      </c>
-      <c r="F13" s="33" t="n">
+      <c r="E13" s="37" t="n">
+        <v>21796.73</v>
+      </c>
+      <c r="F13" s="37" t="n">
         <v>22244.25</v>
       </c>
-      <c r="G13" s="33">
-        <f>IFERROR((F13-E13)*100/E13,0)</f>
-        <v/>
-      </c>
-      <c r="H13" s="38" t="n">
-        <v>70366.78685100001</v>
-      </c>
-      <c r="I13" s="33">
-        <f>IFERROR(H13*100/$E$21,0)</f>
+      <c r="G13" s="43">
+        <f>IFERROR((F13-E13)/E13,0)</f>
+        <v/>
+      </c>
+      <c r="H13" s="41" t="n">
+        <v>-15483.67941</v>
+      </c>
+      <c r="I13" s="43">
+        <f>IFERROR(H13/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -986,21 +980,21 @@
       </c>
       <c r="C14" s="26" t="n"/>
       <c r="D14" s="33" t="n"/>
-      <c r="E14" s="33" t="n">
-        <v>14.66</v>
-      </c>
-      <c r="F14" s="33" t="n">
+      <c r="E14" s="37" t="n">
+        <v>9.609999999999999</v>
+      </c>
+      <c r="F14" s="37" t="n">
         <v>8.76</v>
       </c>
-      <c r="G14" s="33">
-        <f>IFERROR((F14-E14)*100/E14,0)</f>
-        <v/>
-      </c>
-      <c r="H14" s="38" t="n">
-        <v>-24970.68653913</v>
-      </c>
-      <c r="I14" s="33">
-        <f>IFERROR(H14*100/$E$21,0)</f>
+      <c r="G14" s="43">
+        <f>IFERROR((F14-E14)/E14,0)</f>
+        <v/>
+      </c>
+      <c r="H14" s="41" t="n">
+        <v>-7843.732152129999</v>
+      </c>
+      <c r="I14" s="43">
+        <f>IFERROR(H14/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -1012,21 +1006,21 @@
       </c>
       <c r="C15" s="26" t="n"/>
       <c r="D15" s="33" t="n"/>
-      <c r="E15" s="33" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="F15" s="33" t="n">
+      <c r="E15" s="37" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F15" s="37" t="n">
         <v>7.1</v>
       </c>
-      <c r="G15" s="33">
-        <f>IFERROR((F15-E15)*100/E15,0)</f>
-        <v/>
-      </c>
-      <c r="H15" s="38" t="n">
-        <v>-9960.124459900002</v>
-      </c>
-      <c r="I15" s="33">
-        <f>IFERROR(H15*100/$E$21,0)</f>
+      <c r="G15" s="43">
+        <f>IFERROR((F15-E15)/E15,0)</f>
+        <v/>
+      </c>
+      <c r="H15" s="41" t="n">
+        <v>-9860.760068600001</v>
+      </c>
+      <c r="I15" s="43">
+        <f>IFERROR(H15/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -1038,21 +1032,21 @@
       </c>
       <c r="C16" s="26" t="n"/>
       <c r="D16" s="33" t="n"/>
-      <c r="E16" s="33" t="n">
-        <v/>
-      </c>
-      <c r="F16" s="33" t="n">
-        <v/>
-      </c>
-      <c r="G16" s="33">
-        <f>IFERROR((F16-E16)*100/E16,0)</f>
-        <v/>
-      </c>
-      <c r="H16" s="38" t="n">
+      <c r="E16" s="37" t="n">
+        <v/>
+      </c>
+      <c r="F16" s="37" t="n">
+        <v/>
+      </c>
+      <c r="G16" s="43">
+        <f>IFERROR((F16-E16)/E16,0)</f>
+        <v/>
+      </c>
+      <c r="H16" s="41" t="n">
         <v>-37250.43463</v>
       </c>
-      <c r="I16" s="33">
-        <f>IFERROR(H16*100/$E$21,0)</f>
+      <c r="I16" s="43">
+        <f>IFERROR(H16/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -1064,21 +1058,21 @@
       </c>
       <c r="C17" s="26" t="n"/>
       <c r="D17" s="33" t="n"/>
-      <c r="E17" s="33" t="n">
+      <c r="E17" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="33" t="n">
+      <c r="F17" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="G17" s="33">
-        <f>IFERROR((F17-E17)*100/E17,0)</f>
-        <v/>
-      </c>
-      <c r="H17" s="38" t="n">
+      <c r="G17" s="43">
+        <f>IFERROR((F17-E17)/E17,0)</f>
+        <v/>
+      </c>
+      <c r="H17" s="41" t="n">
         <v>10256.11504</v>
       </c>
-      <c r="I17" s="33">
-        <f>IFERROR(H17*100/$E$21,0)</f>
+      <c r="I17" s="43">
+        <f>IFERROR(H17/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -1090,21 +1084,21 @@
       </c>
       <c r="C18" s="26" t="n"/>
       <c r="D18" s="33" t="n"/>
-      <c r="E18" s="33" t="n">
+      <c r="E18" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="33" t="n">
+      <c r="F18" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="33">
-        <f>IFERROR((F18-E18)*100/E18,0)</f>
-        <v/>
-      </c>
-      <c r="H18" s="38" t="n">
+      <c r="G18" s="43">
+        <f>IFERROR((F18-E18)/E18,0)</f>
+        <v/>
+      </c>
+      <c r="H18" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="33">
-        <f>IFERROR(H18*100/$E$21,0)</f>
+      <c r="I18" s="43">
+        <f>IFERROR(H18/$E$21,0)</f>
         <v/>
       </c>
     </row>
@@ -1115,39 +1109,41 @@
         </is>
       </c>
       <c r="C19" s="29" t="n"/>
-      <c r="D19" s="39" t="n"/>
-      <c r="E19" s="39" t="n"/>
-      <c r="F19" s="39" t="n"/>
-      <c r="G19" s="39">
-        <f>IFERROR((F19-E19)*100/E19,0)</f>
-        <v/>
-      </c>
-      <c r="H19" s="45" t="n"/>
-      <c r="I19" s="39">
-        <f>IFERROR(H19*100/$E$21,0)</f>
+      <c r="D19" s="30" t="n"/>
+      <c r="E19" s="38" t="n"/>
+      <c r="F19" s="38" t="n"/>
+      <c r="G19" s="44">
+        <f>IFERROR((F19-E19)/E19,0)</f>
+        <v/>
+      </c>
+      <c r="H19" s="42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="44">
+        <f>IFERROR(H19/$E$21,0)</f>
         <v/>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="20" s="2" thickTop="1">
-      <c r="B20" s="41" t="inlineStr">
+      <c r="B20" s="34" t="inlineStr">
         <is>
           <t>Total Modeled Ridership</t>
         </is>
       </c>
-      <c r="C20" s="42" t="n"/>
-      <c r="D20" s="44" t="n"/>
-      <c r="E20" s="44" t="n">
-        <v>655298.1175000001</v>
-      </c>
-      <c r="F20" s="44" t="n">
+      <c r="C20" s="35" t="n"/>
+      <c r="D20" s="36" t="n"/>
+      <c r="E20" s="39" t="n">
+        <v>805542.9296</v>
+      </c>
+      <c r="F20" s="39" t="n">
         <v>859716.3829999999</v>
       </c>
-      <c r="G20" s="44">
-        <f>IFERROR((F20-E20)*100/E20,0)</f>
-        <v/>
-      </c>
-      <c r="H20" s="44" t="n"/>
-      <c r="I20" s="44">
+      <c r="G20" s="45">
+        <f>IFERROR((F20-E20)/E20,0)</f>
+        <v/>
+      </c>
+      <c r="H20" s="39" t="n"/>
+      <c r="I20" s="45">
         <f>G20</f>
         <v/>
       </c>
@@ -1159,19 +1155,19 @@
         </is>
       </c>
       <c r="C21" s="29" t="n"/>
-      <c r="D21" s="39" t="n"/>
-      <c r="E21" s="39" t="n">
-        <v>628324</v>
-      </c>
-      <c r="F21" s="39" t="n">
+      <c r="D21" s="30" t="n"/>
+      <c r="E21" s="38" t="n">
+        <v>1017648</v>
+      </c>
+      <c r="F21" s="38" t="n">
         <v>739896</v>
       </c>
-      <c r="G21" s="33">
-        <f>IFERROR((F21-E21)*100/E21,0)</f>
-        <v/>
-      </c>
-      <c r="H21" s="39" t="n"/>
-      <c r="I21" s="39">
+      <c r="G21" s="43">
+        <f>IFERROR((F21-E21)/E21,0)</f>
+        <v/>
+      </c>
+      <c r="H21" s="38" t="n"/>
+      <c r="I21" s="44">
         <f>G21</f>
         <v/>
       </c>
@@ -1182,13 +1178,13 @@
           <t>Unexplained Change</t>
         </is>
       </c>
-      <c r="C22" s="40" t="n"/>
-      <c r="D22" s="40" t="n"/>
+      <c r="C22" s="32" t="n"/>
+      <c r="D22" s="32" t="n"/>
       <c r="E22" s="40" t="n"/>
       <c r="F22" s="40" t="n"/>
-      <c r="G22" s="40" t="n"/>
+      <c r="G22" s="32" t="n"/>
       <c r="H22" s="40" t="n"/>
-      <c r="I22" s="40" t="n"/>
+      <c r="I22" s="32" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="23" s="2" thickTop="1"/>
   </sheetData>
@@ -1261,7 +1257,7 @@
       <c r="B4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="E5" s="37" t="inlineStr">
+      <c r="E5" s="49" t="inlineStr">
         <is>
           <t>Average Values</t>
         </is>

</xml_diff>